<commit_message>
Update xlsx package version due to security vulnerability
</commit_message>
<xml_diff>
--- a/knn_classifier/knn_classifier_inputs.xlsx
+++ b/knn_classifier/knn_classifier_inputs.xlsx
@@ -15,15 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
   <si>
     <t>x</t>
   </si>
   <si>
     <t>y</t>
-  </si>
-  <si>
-    <t>Z</t>
   </si>
   <si>
     <t>z</t>
@@ -472,10 +469,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25" customFormat="1" s="1">

</xml_diff>